<commit_message>
update examples- Dam model
</commit_message>
<xml_diff>
--- a/Examples/AHP_Dam/damModel_Excel_FilledIn.xlsx
+++ b/Examples/AHP_Dam/damModel_Excel_FilledIn.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitCODE\cdfAHPANPLib\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shared/GITHUB/AhpAnpLib/Examples/AHP_Dam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1991075-62CF-4DCA-B147-C0B67E0E62F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1439B805-F178-204F-A761-609F5220CD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="915" windowWidth="14430" windowHeight="14415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="920" windowWidth="14440" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pairwise_comp" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="40">
   <si>
     <t>Choose dam level</t>
-  </si>
-  <si>
-    <t>Enter judgments for the paiwise comparisons in the matrix or direct values in the green cells</t>
   </si>
   <si>
     <t>2Decision Criteria</t>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>Half-full dam</t>
+  </si>
+  <si>
+    <t>Enter pairwise comparisons in the white cells of the table or numerical data in the green cells. For the Direct Values column, if the smallest value is best, invert the value before entering it (e.g., $10 as =1/10) .</t>
   </si>
 </sst>
 </file>
@@ -656,54 +656,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J214" sqref="J214"/>
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A221" sqref="A221"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="21" width="15.7109375" customWidth="1"/>
+    <col min="1" max="21" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="6">
         <v>1</v>
@@ -723,9 +723,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="9" t="e">
         <f>1/C4</f>
@@ -748,9 +748,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="9" t="e">
         <f>1/D4</f>
@@ -776,9 +776,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="9" t="e">
         <f>1/E4</f>
@@ -807,9 +807,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="11" t="e">
         <f>SUM(B4:B7)</f>
@@ -832,57 +832,57 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G9" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="11" t="e">
         <f>((MMULT(B8:E8,H4:H7)-4)/(4-1))/0.89</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="H12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B13" s="6">
         <v>1</v>
@@ -903,9 +903,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="9" t="e">
         <f>1/C13</f>
@@ -929,9 +929,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="9" t="e">
         <f>1/D13</f>
@@ -958,9 +958,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="9" t="e">
         <f>1/E13</f>
@@ -990,9 +990,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="9" t="e">
         <f>1/F13</f>
@@ -1025,9 +1025,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="11" t="e">
         <f>SUM(B13:B17)</f>
@@ -1054,57 +1054,57 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H19" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I19" s="11" t="e">
         <f>((MMULT(B18:F18,I13:I17)-5)/(5-1))/1.12</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="G22" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" s="6">
         <v>1</v>
@@ -1125,9 +1125,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="9" t="e">
         <f>1/C23</f>
@@ -1151,9 +1151,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" s="9" t="e">
         <f>1/D23</f>
@@ -1180,9 +1180,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="9" t="e">
         <f>1/E23</f>
@@ -1212,9 +1212,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B27" s="9" t="e">
         <f>1/F23</f>
@@ -1247,9 +1247,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="11" t="e">
         <f>SUM(B23:B27)</f>
@@ -1276,57 +1276,57 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H29" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I29" s="11" t="e">
         <f>((MMULT(B28:F28,I23:I27)-5)/(5-1))/1.12</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="G32" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B33" s="6">
         <v>1</v>
@@ -1347,9 +1347,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B34" s="9" t="e">
         <f>1/C33</f>
@@ -1373,9 +1373,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B35" s="9" t="e">
         <f>1/D33</f>
@@ -1402,9 +1402,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" s="9" t="e">
         <f>1/E33</f>
@@ -1434,9 +1434,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B37" s="9" t="e">
         <f>1/F33</f>
@@ -1469,9 +1469,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" s="11" t="e">
         <f>SUM(B33:B37)</f>
@@ -1498,57 +1498,57 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="H39" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I39" s="11" t="e">
         <f>((MMULT(B38:F38,I33:I37)-5)/(5-1))/1.12</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H42" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="I42" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B43" s="6">
         <v>1</v>
@@ -1569,9 +1569,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B44" s="9" t="e">
         <f>1/C43</f>
@@ -1595,9 +1595,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B45" s="9" t="e">
         <f>1/D43</f>
@@ -1624,9 +1624,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B46" s="9" t="e">
         <f>1/E43</f>
@@ -1656,9 +1656,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" s="9" t="e">
         <f>1/F43</f>
@@ -1691,9 +1691,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" s="11" t="e">
         <f>SUM(B43:B47)</f>
@@ -1720,60 +1720,60 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H49" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I49" s="11" t="e">
         <f>((MMULT(B48:F48,I43:I47)-5)/(5-1))/1.12</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="C52" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="F52" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="4" t="s">
+      <c r="G52" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G52" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="H52" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I52" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J52" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J52" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B53" s="6">
         <v>1</v>
@@ -1795,9 +1795,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B54" s="9" t="e">
         <f>1/C53</f>
@@ -1822,9 +1822,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B55" s="9" t="e">
         <f>1/D53</f>
@@ -1852,9 +1852,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B56" s="9" t="e">
         <f>1/E53</f>
@@ -1885,9 +1885,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B57" s="9" t="e">
         <f>1/F53</f>
@@ -1921,9 +1921,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B58" s="9" t="e">
         <f>1/G53</f>
@@ -1960,9 +1960,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B59" s="11" t="e">
         <f t="shared" ref="B59:G59" si="1">SUM(B53:B58)</f>
@@ -1993,60 +1993,60 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I60" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J60" s="11" t="e">
         <f>((MMULT(B59:G59,J53:J58)-6)/(6-1))/1.25</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="D63" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="E63" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E63" s="4" t="s">
+      <c r="F63" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F63" s="4" t="s">
+      <c r="G63" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G63" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="H63" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I63" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J63" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J63" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B64" s="6">
         <v>1</v>
@@ -2068,9 +2068,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B65" s="9" t="e">
         <f>1/C64</f>
@@ -2095,9 +2095,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B66" s="9" t="e">
         <f>1/D64</f>
@@ -2125,9 +2125,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B67" s="9" t="e">
         <f>1/E64</f>
@@ -2158,9 +2158,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B68" s="9" t="e">
         <f>1/F64</f>
@@ -2194,9 +2194,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B69" s="9" t="e">
         <f>1/G64</f>
@@ -2233,9 +2233,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B70" s="11" t="e">
         <f t="shared" ref="B70:G70" si="3">SUM(B64:B69)</f>
@@ -2266,60 +2266,60 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I71" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J71" s="11" t="e">
         <f>((MMULT(B70:G70,J64:J69)-6)/(6-1))/1.25</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="D74" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="E74" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="F74" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F74" s="4" t="s">
+      <c r="G74" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G74" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="H74" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I74" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J74" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J74" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B75" s="6">
         <v>1</v>
@@ -2341,9 +2341,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B76" s="9" t="e">
         <f>1/C75</f>
@@ -2368,9 +2368,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B77" s="9" t="e">
         <f>1/D75</f>
@@ -2398,9 +2398,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B78" s="9" t="e">
         <f>1/E75</f>
@@ -2431,9 +2431,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B79" s="9" t="e">
         <f>1/F75</f>
@@ -2467,9 +2467,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B80" s="9" t="e">
         <f>1/G75</f>
@@ -2506,9 +2506,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B81" s="11" t="e">
         <f t="shared" ref="B81:G81" si="5">SUM(B75:B80)</f>
@@ -2539,60 +2539,60 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I82" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J82" s="11" t="e">
         <f>((MMULT(B81:G81,J75:J80)-6)/(6-1))/1.25</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="C85" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="D85" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D85" s="4" t="s">
+      <c r="E85" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E85" s="4" t="s">
+      <c r="F85" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F85" s="4" t="s">
+      <c r="G85" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G85" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="H85" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I85" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J85" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J85" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B86" s="6">
         <v>1</v>
@@ -2614,9 +2614,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B87" s="9" t="e">
         <f>1/C86</f>
@@ -2641,9 +2641,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B88" s="9" t="e">
         <f>1/D86</f>
@@ -2671,9 +2671,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B89" s="9" t="e">
         <f>1/E86</f>
@@ -2704,9 +2704,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B90" s="9" t="e">
         <f>1/F86</f>
@@ -2740,9 +2740,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B91" s="9" t="e">
         <f>1/G86</f>
@@ -2779,9 +2779,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B92" s="11" t="e">
         <f t="shared" ref="B92:G92" si="7">SUM(B86:B91)</f>
@@ -2812,60 +2812,60 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I93" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J93" s="11" t="e">
         <f>((MMULT(B92:G92,J86:J91)-6)/(6-1))/1.25</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+      <c r="B96" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="C96" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="D96" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="E96" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E96" s="4" t="s">
+      <c r="F96" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F96" s="4" t="s">
+      <c r="G96" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G96" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="H96" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J96" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J96" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B97" s="6">
         <v>1</v>
@@ -2887,9 +2887,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B98" s="9" t="e">
         <f>1/C97</f>
@@ -2914,9 +2914,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B99" s="9" t="e">
         <f>1/D97</f>
@@ -2944,9 +2944,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B100" s="9" t="e">
         <f>1/E97</f>
@@ -2977,9 +2977,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B101" s="9" t="e">
         <f>1/F97</f>
@@ -3013,9 +3013,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B102" s="9" t="e">
         <f>1/G97</f>
@@ -3052,9 +3052,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B103" s="11" t="e">
         <f t="shared" ref="B103:G103" si="9">SUM(B97:B102)</f>
@@ -3085,54 +3085,54 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I104" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J104" s="11" t="e">
         <f>((MMULT(B103:G103,J97:J102)-6)/(6-1))/1.25</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" ht="21" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B107" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="C107" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="D107" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="E107" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E107" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F107" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G107" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H107" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H107" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B108" s="6">
         <v>1</v>
@@ -3152,9 +3152,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B109" s="9" t="e">
         <f>1/C108</f>
@@ -3177,9 +3177,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B110" s="9" t="e">
         <f>1/D108</f>
@@ -3205,9 +3205,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B111" s="9" t="e">
         <f>1/E108</f>
@@ -3236,9 +3236,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B112" s="11" t="e">
         <f>SUM(B108:B111)</f>
@@ -3261,54 +3261,54 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G113" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H113" s="11" t="e">
         <f>((MMULT(B112:E112,H108:H111)-4)/(4-1))/0.89</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B116" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="C116" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="D116" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D116" s="4" t="s">
+      <c r="E116" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E116" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F116" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G116" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H116" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H116" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B117" s="6">
         <v>1</v>
@@ -3328,9 +3328,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B118" s="9" t="e">
         <f>1/C117</f>
@@ -3353,9 +3353,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B119" s="9" t="e">
         <f>1/D117</f>
@@ -3381,9 +3381,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B120" s="9" t="e">
         <f>1/E117</f>
@@ -3412,9 +3412,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B121" s="11" t="e">
         <f>SUM(B117:B120)</f>
@@ -3437,54 +3437,54 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G122" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H122" s="11" t="e">
         <f>((MMULT(B121:E121,H117:H120)-4)/(4-1))/0.89</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B125" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="C125" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C125" s="4" t="s">
+      <c r="D125" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D125" s="4" t="s">
+      <c r="E125" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E125" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F125" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G125" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H125" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H125" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B126" s="6">
         <v>1</v>
@@ -3504,9 +3504,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B127" s="9" t="e">
         <f>1/C126</f>
@@ -3529,9 +3529,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B128" s="9" t="e">
         <f>1/D126</f>
@@ -3557,9 +3557,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B129" s="9" t="e">
         <f>1/E126</f>
@@ -3588,9 +3588,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B130" s="11" t="e">
         <f>SUM(B126:B129)</f>
@@ -3613,54 +3613,54 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G131" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H131" s="11" t="e">
         <f>((MMULT(B130:E130,H126:H129)-4)/(4-1))/0.89</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B134" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="C134" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="D134" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D134" s="4" t="s">
+      <c r="E134" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E134" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F134" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G134" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H134" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H134" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B135" s="6">
         <v>1</v>
@@ -3680,9 +3680,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B136" s="9" t="e">
         <f>1/C135</f>
@@ -3705,9 +3705,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B137" s="9" t="e">
         <f>1/D135</f>
@@ -3733,9 +3733,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B138" s="9" t="e">
         <f>1/E135</f>
@@ -3764,9 +3764,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B139" s="11" t="e">
         <f>SUM(B135:B138)</f>
@@ -3789,54 +3789,54 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G140" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H140" s="11" t="e">
         <f>((MMULT(B139:E139,H135:H138)-4)/(4-1))/0.89</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B143" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="C143" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C143" s="4" t="s">
+      <c r="D143" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D143" s="4" t="s">
+      <c r="E143" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E143" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F143" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G143" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H143" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H143" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B144" s="6">
         <v>1</v>
@@ -3856,9 +3856,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B145" s="9" t="e">
         <f>1/C144</f>
@@ -3881,9 +3881,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B146" s="9" t="e">
         <f>1/D144</f>
@@ -3909,9 +3909,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B147" s="9" t="e">
         <f>1/E144</f>
@@ -3940,9 +3940,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B148" s="11" t="e">
         <f>SUM(B144:B147)</f>
@@ -3965,54 +3965,54 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G149" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H149" s="11" t="e">
         <f>((MMULT(B148:E148,H144:H147)-4)/(4-1))/0.89</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A152" s="3" t="s">
+      <c r="B152" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B152" s="4" t="s">
+      <c r="C152" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C152" s="4" t="s">
+      <c r="D152" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D152" s="4" t="s">
+      <c r="E152" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E152" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F152" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G152" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H152" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H152" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B153" s="6">
         <v>1</v>
@@ -4032,9 +4032,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B154" s="9" t="e">
         <f>1/C153</f>
@@ -4057,9 +4057,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B155" s="9" t="e">
         <f>1/D153</f>
@@ -4085,9 +4085,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B156" s="9" t="e">
         <f>1/E153</f>
@@ -4116,9 +4116,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B157" s="11" t="e">
         <f>SUM(B153:B156)</f>
@@ -4141,48 +4141,48 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G158" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H158" s="11" t="e">
         <f>((MMULT(B157:E157,H153:H156)-4)/(4-1))/0.89</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B161" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="C161" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C161" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="D161" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E161" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F161" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F161" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B162" s="6">
         <v>1</v>
@@ -4200,9 +4200,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B163" s="9" t="e">
         <f>1/C162</f>
@@ -4223,9 +4223,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B164" s="11" t="e">
         <f>SUM(B162:B163)</f>
@@ -4240,48 +4240,48 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E165" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F165" s="11" t="e">
         <f>((MMULT(B164:C164,F162:F163)-2)/(2-1))/1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="166" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B168" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C168" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C168" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="D168" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E168" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F168" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F168" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B169" s="6">
         <v>1</v>
@@ -4299,9 +4299,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B170" s="9" t="e">
         <f>1/C169</f>
@@ -4322,9 +4322,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B171" s="11" t="e">
         <f>SUM(B169:B170)</f>
@@ -4339,45 +4339,45 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E172" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F172" s="11" t="e">
         <f>((MMULT(B171:C171,F169:F170)-2)/(2-1))/1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="173" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D175" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E175" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E175" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B176" s="6">
         <v>1</v>
@@ -4394,9 +4394,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B177" s="11">
         <f>SUM(B176:B176)</f>
@@ -4407,45 +4407,45 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D178" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E178" s="11" t="e">
         <f>((MMULT(B177:B177,E176:E176)-1)/(1-1))/1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="179" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="B181" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D181" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E181" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E181" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B182" s="6">
         <v>1</v>
@@ -4462,9 +4462,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B183" s="11">
         <f>SUM(B182:B182)</f>
@@ -4475,48 +4475,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D184" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E184" s="11" t="e">
         <f>((MMULT(B183:B183,E182:E182)-1)/(1-1))/1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B187" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B187" s="4" t="s">
+      <c r="C187" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C187" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D187" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E187" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F187" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F187" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B188" s="6">
         <v>1</v>
@@ -4534,9 +4534,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B189" s="9" t="e">
         <f>1/C188</f>
@@ -4557,9 +4557,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B190" s="11" t="e">
         <f>SUM(B188:B189)</f>
@@ -4574,48 +4574,48 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E191" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F191" s="11" t="e">
         <f>((MMULT(B190:C190,F188:F189)-2)/(2-1))/1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B194" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="C194" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C194" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D194" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E194" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F194" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F194" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B195" s="6">
         <v>1</v>
@@ -4633,9 +4633,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B196" s="9" t="e">
         <f>1/C195</f>
@@ -4656,9 +4656,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B197" s="11" t="e">
         <f>SUM(B195:B196)</f>
@@ -4673,48 +4673,48 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E198" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F198" s="11" t="e">
         <f>((MMULT(B197:C197,F195:F196)-2)/(2-1))/1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="199" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B201" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B201" s="4" t="s">
+      <c r="C201" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C201" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D201" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E201" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F201" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F201" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B202" s="6">
         <v>1</v>
@@ -4732,9 +4732,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B203" s="9" t="e">
         <f>1/C202</f>
@@ -4755,9 +4755,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B204" s="11" t="e">
         <f>SUM(B202:B203)</f>
@@ -4772,48 +4772,48 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E205" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F205" s="11" t="e">
         <f>((MMULT(B204:C204,F202:F203)-2)/(2-1))/1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="206" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B208" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B208" s="4" t="s">
+      <c r="C208" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C208" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D208" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E208" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F208" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F208" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B209" s="6">
         <v>1</v>
@@ -4831,9 +4831,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B210" s="9" t="e">
         <f>1/C209</f>
@@ -4854,9 +4854,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B211" s="11" t="e">
         <f>SUM(B209:B210)</f>
@@ -4871,48 +4871,48 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E212" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F212" s="11" t="e">
         <f>((MMULT(B211:C211,F209:F210)-2)/(2-1))/1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="213" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B215" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B215" s="4" t="s">
+      <c r="C215" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C215" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D215" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E215" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F215" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F215" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B216" s="6">
         <v>1</v>
@@ -4930,9 +4930,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B217" s="9" t="e">
         <f>1/C216</f>
@@ -4953,9 +4953,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B218" s="11" t="e">
         <f>SUM(B216:B217)</f>
@@ -4970,48 +4970,48 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E219" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F219" s="11" t="e">
         <f>((MMULT(B218:C218,F216:F217)-2)/(2-1))/1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="220" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A221" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A222" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A221" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A222" s="3" t="s">
+      <c r="B222" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B222" s="4" t="s">
+      <c r="C222" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C222" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="D222" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E222" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F222" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F222" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B223" s="6">
         <v>1</v>
@@ -5029,9 +5029,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B224" s="9" t="e">
         <f>1/C223</f>
@@ -5052,9 +5052,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B225" s="11" t="e">
         <f>SUM(B223:B224)</f>
@@ -5069,9 +5069,9 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E226" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F226" s="11" t="e">
         <f>((MMULT(B225:C225,F223:F224)-2)/(2-1))/1</f>

</xml_diff>